<commit_message>
update neqsim dll for distribution to IT created
</commit_message>
<xml_diff>
--- a/NeqSimExcel/NeqSimExcel.xlsx
+++ b/NeqSimExcel/NeqSimExcel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15690" windowHeight="6210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12705" windowHeight="6615"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="18" r:id="rId1"/>
@@ -1130,9 +1130,6 @@
     <t>Select HYSYS fluid package to import</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>sulfur(S8)</t>
   </si>
   <si>
@@ -1239,6 +1236,9 @@
   </si>
   <si>
     <t>OLGA fluid property table</t>
+  </si>
+  <si>
+    <t>Enter fluid name:</t>
   </si>
 </sst>
 </file>
@@ -1393,7 +1393,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1598,6 +1598,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1611,7 +1626,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1766,6 +1781,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -7091,15 +7107,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>247650</xdr:colOff>
+          <xdr:colOff>285750</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>628650</xdr:colOff>
+          <xdr:colOff>666750</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -8155,15 +8171,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>1085850</xdr:colOff>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -10991,9 +11007,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11004,7 +11018,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="64" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -11072,7 +11086,7 @@
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="67" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11107,7 +11121,7 @@
     </row>
     <row r="23" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="67" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11155,17 +11169,17 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="67" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="67" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="67" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
@@ -11219,7 +11233,7 @@
     <hyperlink ref="A22" location="AddPseudo!A1" display="Add psedocomponents"/>
     <hyperlink ref="A36" location="ReadFluid!A1" display="Import fluid"/>
     <hyperlink ref="A23" location="wellstream!A1" display="GOR/k-value to well stream"/>
-    <hyperlink ref="A16" location="'Water, ice and hydrate T'!A1" display="Water dew point"/>
+    <hyperlink ref="A16" location="'Water dew point'!A1" display="Water dew point"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="598" r:id="rId2"/>
@@ -11475,9 +11489,7 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -11493,7 +11505,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11789,7 +11801,7 @@
         <v>54</v>
       </c>
       <c r="F1" s="83" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G1" s="84" t="s">
         <v>19</v>
@@ -11800,7 +11812,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F2" s="86" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G2" s="41">
         <v>40</v>
@@ -11811,7 +11823,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F3" s="86" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G3" s="41">
         <v>15</v>
@@ -11822,7 +11834,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F4" s="86" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G4" s="41">
         <v>1.01325</v>
@@ -11844,7 +11856,7 @@
         <v>150</v>
       </c>
       <c r="H6" s="89" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -11980,7 +11992,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12063,7 +12077,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12432,7 +12446,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12562,8 +12576,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12575,7 +12589,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -12586,10 +12600,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
+        <v>338</v>
+      </c>
+      <c r="B5" t="s">
         <v>339</v>
-      </c>
-      <c r="B5" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -12599,15 +12613,15 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>313</v>
-      </c>
-      <c r="B20" t="s">
-        <v>325</v>
+        <v>349</v>
+      </c>
+      <c r="B20" s="102" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -12731,9 +12745,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R116"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12804,7 +12816,7 @@
       </c>
       <c r="P2" s="34"/>
       <c r="R2" s="99" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -12961,13 +12973,13 @@
       </c>
       <c r="L9" s="20"/>
       <c r="O9" s="33" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P9" s="34"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="94" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B10" s="94">
         <v>0</v>
@@ -13039,7 +13051,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="94" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B13" s="94">
         <v>0</v>
@@ -13055,7 +13067,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="94" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B14" s="94">
         <v>0</v>
@@ -13071,7 +13083,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="94" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B15" s="94">
         <v>0</v>
@@ -13085,7 +13097,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="94" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B16" s="94">
         <v>0</v>
@@ -13097,7 +13109,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="94" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B17" s="94">
         <v>0</v>
@@ -13175,7 +13187,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="98" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B23" s="94">
         <v>0</v>
@@ -13211,7 +13223,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="98" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B26" s="94">
         <v>0</v>
@@ -14417,7 +14429,7 @@
     </row>
     <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B114" s="29">
         <v>0</v>
@@ -14428,7 +14440,7 @@
     </row>
     <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B115" s="29">
         <v>0</v>
@@ -14564,15 +14576,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>8</xdr:col>
-                <xdr:colOff>247650</xdr:colOff>
+                <xdr:colOff>285750</xdr:colOff>
                 <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>8</xdr:col>
-                <xdr:colOff>628650</xdr:colOff>
+                <xdr:colOff>666750</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -14685,7 +14697,7 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1041" r:id="rId22" name="_ActiveXWrapper15">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>10</xdr:col>
@@ -14709,8 +14721,8 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1040" r:id="rId24" name="_ActiveXWrapper14">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId25">
+        <control shapeId="1040" r:id="rId23" name="_ActiveXWrapper14">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId24">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>10</xdr:col>
@@ -14729,13 +14741,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1040" r:id="rId24" name="_ActiveXWrapper14"/>
+        <control shapeId="1040" r:id="rId23" name="_ActiveXWrapper14"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId26" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId27">
+        <control shapeId="1026" r:id="rId25" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId26">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -14754,13 +14766,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId26" name="_ActiveXWrapper1"/>
+        <control shapeId="1026" r:id="rId25" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId28" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId29">
+        <control shapeId="1028" r:id="rId27" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId28">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -14779,13 +14791,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId28" name="_ActiveXWrapper3"/>
+        <control shapeId="1028" r:id="rId27" name="_ActiveXWrapper3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId30" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId31">
+        <control shapeId="1029" r:id="rId29" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId30">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -14804,13 +14816,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId30" name="_ActiveXWrapper4"/>
+        <control shapeId="1029" r:id="rId29" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId32" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId33">
+        <control shapeId="1030" r:id="rId31" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -14829,13 +14841,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1030" r:id="rId32" name="_ActiveXWrapper5"/>
+        <control shapeId="1030" r:id="rId31" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1031" r:id="rId34" name="_ActiveXWrapper6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId35">
+        <control shapeId="1031" r:id="rId33" name="_ActiveXWrapper6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId34">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
@@ -14854,13 +14866,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1031" r:id="rId34" name="_ActiveXWrapper6"/>
+        <control shapeId="1031" r:id="rId33" name="_ActiveXWrapper6"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId36" name="_ActiveXWrapper13">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId37">
+        <control shapeId="1032" r:id="rId35" name="_ActiveXWrapper13">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId36">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -14879,13 +14891,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1032" r:id="rId36" name="_ActiveXWrapper13"/>
+        <control shapeId="1032" r:id="rId35" name="_ActiveXWrapper13"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId38" name="_ActiveXWrapper7">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId39">
+        <control shapeId="1033" r:id="rId37" name="_ActiveXWrapper7">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId38">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -14904,13 +14916,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1033" r:id="rId38" name="_ActiveXWrapper7"/>
+        <control shapeId="1033" r:id="rId37" name="_ActiveXWrapper7"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1034" r:id="rId40" name="_ActiveXWrapper8">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId41">
+        <control shapeId="1034" r:id="rId39" name="_ActiveXWrapper8">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId40">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>7</xdr:col>
@@ -14929,13 +14941,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1034" r:id="rId40" name="_ActiveXWrapper8"/>
+        <control shapeId="1034" r:id="rId39" name="_ActiveXWrapper8"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId42" name="_ActiveXWrapper9">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId43">
+        <control shapeId="1035" r:id="rId41" name="_ActiveXWrapper9">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId42">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>7</xdr:col>
@@ -14954,13 +14966,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1035" r:id="rId42" name="_ActiveXWrapper9"/>
+        <control shapeId="1035" r:id="rId41" name="_ActiveXWrapper9"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId44" name="_ActiveXWrapper10">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId45">
+        <control shapeId="1036" r:id="rId43" name="_ActiveXWrapper10">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId44">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -14979,13 +14991,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1036" r:id="rId44" name="_ActiveXWrapper10"/>
+        <control shapeId="1036" r:id="rId43" name="_ActiveXWrapper10"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1037" r:id="rId46" name="_ActiveXWrapper11">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId47">
+        <control shapeId="1037" r:id="rId45" name="_ActiveXWrapper11">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId46">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -15004,13 +15016,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1037" r:id="rId46" name="_ActiveXWrapper11"/>
+        <control shapeId="1037" r:id="rId45" name="_ActiveXWrapper11"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1038" r:id="rId48" name="_ActiveXWrapper12">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId25">
+        <control shapeId="1038" r:id="rId47" name="_ActiveXWrapper12">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId24">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -15029,13 +15041,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1038" r:id="rId48" name="_ActiveXWrapper12"/>
+        <control shapeId="1038" r:id="rId47" name="_ActiveXWrapper12"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1039" r:id="rId49" name="_ActiveXWrapper27">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId50">
+        <control shapeId="1039" r:id="rId48" name="_ActiveXWrapper27">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId49">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>10</xdr:col>
@@ -15054,7 +15066,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1039" r:id="rId49" name="_ActiveXWrapper27"/>
+        <control shapeId="1039" r:id="rId48" name="_ActiveXWrapper27"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -15067,7 +15079,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15092,7 +15104,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
@@ -15216,9 +15228,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15352,9 +15362,7 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15430,22 +15438,22 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -15902,15 +15910,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>28575</xdr:colOff>
                 <xdr:row>8</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:rowOff>123825</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1085850</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>10</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -16004,9 +16012,7 @@
   <sheetPr codeName="Sheet24"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16384,7 +16390,9 @@
   <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16804,7 +16812,9 @@
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17296,9 +17306,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18631,9 +18639,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18818,9 +18824,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18970,9 +18974,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19050,7 +19052,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19156,8 +19158,8 @@
   <sheetPr codeName="Sheet29"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19174,13 +19176,13 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1" t="s">
         <v>334</v>
-      </c>
-      <c r="D1" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
prepare for version 20
</commit_message>
<xml_diff>
--- a/NeqSimExcel/NeqSimExcel.xlsx
+++ b/NeqSimExcel/NeqSimExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app\GITtest5\NeqSimExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esol\OneDrive - Equinor\programming\NeqSim.NET\NeqSimExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{420B4A52-CB6B-4C92-923D-C41B2391BCD9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138EEAF6-DBBB-497B-840F-9812EA9023D2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22680" windowHeight="6105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="18" r:id="rId1"/>
@@ -43,7 +43,15 @@
     <sheet name="DewPointControl" sheetId="28" r:id="rId28"/>
     <sheet name="NeqSimWeb" sheetId="19" r:id="rId29"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1212,9 +1220,6 @@
     <t>fluid name</t>
   </si>
   <si>
-    <t>NeqSim Excel 2018.1</t>
-  </si>
-  <si>
     <t>Database path</t>
   </si>
   <si>
@@ -1240,6 +1245,9 @@
   </si>
   <si>
     <t>Enter fluid name:</t>
+  </si>
+  <si>
+    <t>NeqSim Excel 2.0</t>
   </si>
 </sst>
 </file>
@@ -1247,8 +1255,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1394,7 +1402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1564,43 +1572,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -1618,16 +1589,16 @@
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1776,13 +1747,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1873,6 +1841,23 @@
 
 <file path=xl/activeX/activeX100.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4E43028E041544444F74A6C94396E211329D04"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3493"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="556"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX101.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
@@ -1888,7 +1873,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX101.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX102.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1905,7 +1890,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX102.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX103.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1922,7 +1907,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX103.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX104.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1939,7 +1924,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX104.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX105.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1956,7 +1941,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX105.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX106.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1973,7 +1958,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX106.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX107.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1990,7 +1975,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX107.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX108.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -2007,7 +1992,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX108.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX109.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -2020,23 +2005,6 @@
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="2011"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="423"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX109.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.WebBrowser"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="113D49342179021442F1BA4E1ABBE84341E461"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="36407"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="23178"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -2054,6 +2022,23 @@
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="556"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX110.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.WebBrowser"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="113D49342179021442F1BA4E1ABBE84341E461"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="36407"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="23178"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -2460,8 +2445,8 @@
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="2514"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="450"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4286"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="873"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -3114,17 +3099,17 @@
 
 <file path=xl/activeX/activeX69.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="45D33512E48096441A0497A34BF5576B3AED64"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="9A69B97EF9CE7194164988409DF9892D9BAF59"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4022"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="556"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="2646"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="370"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -3148,6 +3133,23 @@
 
 <file path=xl/activeX/activeX70.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="45D33512E48096441A0497A34BF5576B3AED64"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4022"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="556"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX71.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
@@ -3163,7 +3165,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX72.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3180,7 +3182,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX73.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3197,7 +3199,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX74.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3214,7 +3216,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX75.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3231,7 +3233,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX76.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3248,7 +3250,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX77.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3265,7 +3267,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX78.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3282,29 +3284,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX79.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
   <ax:ocxPr ax:name="Cookie" ax:value="5C510AE1455D9F542EA587FD5E4EC14F5269B5"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4207"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="556"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX79.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="67A6C00D6687E26475C6958E6D14CE9EE21C16"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -3338,7 +3323,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="72271141F7F304743D97A5F1778C4D0587F767"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="67A6C00D6687E26475C6958E6D14CE9EE21C16"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -3355,7 +3340,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="9E13BA6D292D4B946339B3CE90165787BA7C39"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="72271141F7F304743D97A5F1778C4D0587F767"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -3372,7 +3357,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="13E1C5BA71AC7C14A361AD7410D08BDB74F5C1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="9E13BA6D292D4B946339B3CE90165787BA7C39"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -3389,6 +3374,23 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="13E1C5BA71AC7C14A361AD7410D08BDB74F5C1"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4207"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="556"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX84.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
   <ax:ocxPr ax:name="Cookie" ax:value="16D4EADA81744B14F1A18BDE1B0C049C53E8A1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
@@ -3401,7 +3403,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX85.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3418,7 +3420,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX86.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3435,7 +3437,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX87.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3452,7 +3454,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX87.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX88.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3469,7 +3471,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX88.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX89.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3482,23 +3484,6 @@
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="1799"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="741"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX89.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="203310F762F6B524A0B2B83621DE236AA6F882"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="2990"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="556"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -3525,7 +3510,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="17A43E074162A2147ED1B3F91ADBE24223ADC1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="203310F762F6B524A0B2B83621DE236AA6F882"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -3542,6 +3527,23 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="17A43E074162A2147ED1B3F91ADBE24223ADC1"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="2990"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="556"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX92.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
   <ax:ocxPr ax:name="Cookie" ax:value="1BD9DA6BF17560145B618E451B052818D43BF1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
@@ -3554,7 +3556,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX92.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX93.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3571,7 +3573,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX93.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX94.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3588,7 +3590,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX95.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3605,7 +3607,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX95.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX96.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3622,7 +3624,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX96.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX97.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3639,7 +3641,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX97.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX98.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3656,7 +3658,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX98.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX99.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3669,23 +3671,6 @@
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="2328"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="450"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX99.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4E43028E041544444F74A6C94396E211329D04"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3493"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="556"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -5538,6 +5523,68 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>38100</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>990600</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9225" name="_ActiveXWrapper5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9225"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000009240000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -7356,15 +7403,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>17</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>1</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>17</xdr:col>
-          <xdr:colOff>933450</xdr:colOff>
+          <xdr:col>18</xdr:col>
+          <xdr:colOff>590550</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -11008,7 +11055,9 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11019,7 +11068,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="64" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -11170,17 +11219,17 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="67" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="67" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="67" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
@@ -12578,7 +12627,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12619,9 +12668,9 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>349</v>
-      </c>
-      <c r="B20" s="102" t="s">
+        <v>348</v>
+      </c>
+      <c r="B20" s="99" t="s">
         <v>324</v>
       </c>
     </row>
@@ -12737,6 +12786,31 @@
         <control shapeId="9223" r:id="rId10" name="_ActiveXWrapper10"/>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9225" r:id="rId12" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>990600</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9225" r:id="rId12" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </controls>
 </worksheet>
 </file>
@@ -12744,9 +12818,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R116"/>
+  <dimension ref="A1:S116"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12770,7 +12846,7 @@
     <col min="19" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -12787,7 +12863,7 @@
       <c r="L1" s="11"/>
       <c r="M1" s="11"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="94" t="s">
         <v>32</v>
       </c>
@@ -12816,11 +12892,12 @@
         <v>142</v>
       </c>
       <c r="P2" s="34"/>
-      <c r="R2" s="99" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R2" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="S2" s="14"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="94" t="s">
         <v>33</v>
       </c>
@@ -12841,9 +12918,10 @@
       <c r="N3" s="11"/>
       <c r="O3" s="35"/>
       <c r="P3" s="36"/>
-      <c r="R3" s="100"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R3" s="19"/>
+      <c r="S3" s="20"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="94" t="s">
         <v>34</v>
       </c>
@@ -12866,9 +12944,10 @@
       <c r="N4" s="11"/>
       <c r="O4" s="35"/>
       <c r="P4" s="36"/>
-      <c r="R4" s="100"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R4" s="19"/>
+      <c r="S4" s="20"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="94" t="s">
         <v>1</v>
       </c>
@@ -12889,9 +12968,10 @@
       <c r="N5" s="11"/>
       <c r="O5" s="35"/>
       <c r="P5" s="36"/>
-      <c r="R5" s="100"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R5" s="19"/>
+      <c r="S5" s="20"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="94" t="s">
         <v>2</v>
       </c>
@@ -12912,9 +12992,10 @@
       <c r="N6" s="11"/>
       <c r="O6" s="35"/>
       <c r="P6" s="36"/>
-      <c r="R6" s="100"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R6" s="19"/>
+      <c r="S6" s="20"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="94" t="s">
         <v>4</v>
       </c>
@@ -12934,9 +13015,10 @@
       <c r="N7" s="11"/>
       <c r="O7" s="37"/>
       <c r="P7" s="38"/>
-      <c r="R7" s="101"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R7" s="24"/>
+      <c r="S7" s="25"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="94" t="s">
         <v>5</v>
       </c>
@@ -12956,7 +13038,7 @@
       </c>
       <c r="L8" s="14"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="94" t="s">
         <v>6</v>
       </c>
@@ -12978,7 +13060,7 @@
       </c>
       <c r="P9" s="34"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="94" t="s">
         <v>325</v>
       </c>
@@ -12998,7 +13080,7 @@
       <c r="O10" s="35"/>
       <c r="P10" s="36"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="94" t="s">
         <v>7</v>
       </c>
@@ -13024,7 +13106,7 @@
       <c r="O11" s="35"/>
       <c r="P11" s="36"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="94" t="s">
         <v>8</v>
       </c>
@@ -13050,7 +13132,7 @@
       <c r="O12" s="37"/>
       <c r="P12" s="38"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="94" t="s">
         <v>326</v>
       </c>
@@ -13066,7 +13148,7 @@
       <c r="K13" s="27"/>
       <c r="L13" s="28"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="94" t="s">
         <v>327</v>
       </c>
@@ -13082,7 +13164,7 @@
       <c r="K14" s="19"/>
       <c r="L14" s="20"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="94" t="s">
         <v>328</v>
       </c>
@@ -13096,7 +13178,7 @@
       <c r="K15" s="24"/>
       <c r="L15" s="25"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="94" t="s">
         <v>329</v>
       </c>
@@ -15052,15 +15134,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>17</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
+                <xdr:colOff>47625</xdr:colOff>
                 <xdr:row>2</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>17</xdr:col>
-                <xdr:colOff>933450</xdr:colOff>
+                <xdr:col>18</xdr:col>
+                <xdr:colOff>590550</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -15105,7 +15187,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
@@ -15439,7 +15521,7 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15449,12 +15531,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -15748,7 +15830,9 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
updates in neqsim vba
</commit_message>
<xml_diff>
--- a/NeqSimExcel/NeqSimExcel.xlsx
+++ b/NeqSimExcel/NeqSimExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esol\OneDrive - Equinor\programming\NeqSim.NET\NeqSimExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138EEAF6-DBBB-497B-840F-9812EA9023D2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92E8687-259B-4D15-BC26-D18485822D8A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="18" r:id="rId1"/>
@@ -7405,7 +7405,7 @@
           <xdr:col>17</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>18</xdr:col>
@@ -11055,8 +11055,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12626,8 +12626,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12820,9 +12820,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S116"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
update to version 2.4.0
</commit_message>
<xml_diff>
--- a/NeqSimExcel/NeqSimExcel.xlsx
+++ b/NeqSimExcel/NeqSimExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esol\OneDrive - Equinor\programming\NeqSimWin\NeqSimExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://statoilsrm-my.sharepoint.com/personal/esol_equinor_com/Documents/programming/NeqSimWin/NeqSimExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FCA6B4-B0EC-4BEB-8205-0EB1FBEA7891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{4AEA63DF-D9AE-4F7D-A762-3FEF7B21BF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B97D1FFC-527C-49BA-AC38-D105551361BF}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="18" r:id="rId1"/>
@@ -39,8 +39,9 @@
     <sheet name="BinaryCalc" sheetId="29" r:id="rId24"/>
     <sheet name="Valve" sheetId="24" r:id="rId25"/>
     <sheet name="Compressor" sheetId="25" r:id="rId26"/>
-    <sheet name="SepProcess" sheetId="26" r:id="rId27"/>
-    <sheet name="DewPointControl" sheetId="28" r:id="rId28"/>
+    <sheet name="Expander" sheetId="34" r:id="rId27"/>
+    <sheet name="SepProcess" sheetId="26" r:id="rId28"/>
+    <sheet name="DewPointControl" sheetId="28" r:id="rId29"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="351">
   <si>
     <t>Component</t>
   </si>
@@ -1246,10 +1247,13 @@
     <t>Dehydration process</t>
   </si>
   <si>
-    <t>NeqSim Excel 2.2.1</t>
-  </si>
-  <si>
     <t>22,989769</t>
+  </si>
+  <si>
+    <t>Expander</t>
+  </si>
+  <si>
+    <t>NeqSim Excel 2.4.0</t>
   </si>
 </sst>
 </file>
@@ -1846,6 +1850,23 @@
 
 <file path=xl/activeX/activeX100.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="68033A1B56FD05648106B2226A576DF3F7F206"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1990"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="413"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX101.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
@@ -1861,7 +1882,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX101.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX102.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1878,7 +1899,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX102.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX103.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1895,7 +1916,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX103.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX104.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1912,7 +1933,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX104.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX105.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3461,6 +3482,23 @@
 
 <file path=xl/activeX/activeX93.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1AA0A14DD18F2414614189F2114B04B423D361"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="2037"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="688"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX94.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
@@ -3476,7 +3514,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX95.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3493,7 +3531,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX95.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX96.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3510,7 +3548,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX96.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX97.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3527,7 +3565,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX97.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX98.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3544,7 +3582,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX98.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX99.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.LinkLabel"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -3557,23 +3595,6 @@
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="2011"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="423"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX99.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="68033A1B56FD05648106B2226A576DF3F7F206"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1990"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="413"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -8451,6 +8472,73 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>85725</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>819150</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>95250</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="153601" name="_ActiveXWrapper1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s153601"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1A00-000001580200}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing26.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
           <xdr:row>20</xdr:row>
@@ -8470,7 +8558,7 @@
                   <a14:compatExt spid="_x0000_s92161"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1A00-000001680100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000001680100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8532,7 +8620,7 @@
                   <a14:compatExt spid="_x0000_s92162"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1A00-000002680100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000002680100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8594,7 +8682,7 @@
                   <a14:compatExt spid="_x0000_s92163"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1A00-000003680100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000003680100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8656,7 +8744,7 @@
                   <a14:compatExt spid="_x0000_s92164"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1A00-000004680100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000004680100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8718,7 +8806,7 @@
                   <a14:compatExt spid="_x0000_s92165"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1A00-000005680100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000005680100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8775,7 +8863,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1A00-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8824,7 +8912,7 @@
                   <a14:compatExt spid="_x0000_s92166"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1A00-000006680100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000006680100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8866,7 +8954,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing27.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -8891,7 +8979,7 @@
                   <a14:compatExt spid="_x0000_s96257"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000001780100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1C00-000001780100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8953,7 +9041,7 @@
                   <a14:compatExt spid="_x0000_s96258"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000002780100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1C00-000002780100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9015,7 +9103,7 @@
                   <a14:compatExt spid="_x0000_s96259"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000003780100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1C00-000003780100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9077,7 +9165,7 @@
                   <a14:compatExt spid="_x0000_s96260"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000004780100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1C00-000004780100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9139,7 +9227,7 @@
                   <a14:compatExt spid="_x0000_s96261"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000005780100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1C00-000005780100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9201,7 +9289,7 @@
                   <a14:compatExt spid="_x0000_s96262"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000006780100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1C00-000006780100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9258,7 +9346,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1B00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1C00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10581,7 +10669,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -10594,7 +10682,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="64" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -10648,6 +10736,9 @@
     <row r="13" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="67" t="s">
         <v>183</v>
+      </c>
+      <c r="B13" s="63" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10810,6 +10901,7 @@
     <hyperlink ref="A36" location="ReadFluid!A1" display="Import fluid" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
     <hyperlink ref="A23" location="wellstream!A1" display="GOR/k-value to well stream" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="A16" location="'Water dew point'!A1" display="Water dew point" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B13" location="Expander!A1" display="Expander" xr:uid="{817069B4-0A6B-4751-9FA7-C39B4C2FBFA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="598" r:id="rId2"/>
@@ -12245,8 +12337,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13965,7 +14057,7 @@
         <v>0</v>
       </c>
       <c r="C116" s="100" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -15756,9 +15848,7 @@
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15860,6 +15950,114 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725CDA6B-3333-4364-884D-73F56F93A8BB}">
+  <sheetPr codeName="Sheet30"/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="74" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="74">
+        <v>20</v>
+      </c>
+      <c r="B2" s="74">
+        <v>25</v>
+      </c>
+      <c r="C2" s="74">
+        <v>10</v>
+      </c>
+      <c r="D2" s="74">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="74">
+        <v>30</v>
+      </c>
+      <c r="B3" s="74">
+        <v>25</v>
+      </c>
+      <c r="C3" s="74">
+        <v>20</v>
+      </c>
+      <c r="D3" s="74">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="598" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="153601" r:id="rId4" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>85725</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="153601" r:id="rId4" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:H24"/>
@@ -16281,7 +16479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:H28"/>

</xml_diff>